<commit_message>
[MOSIP-19230] Virtual regcenter and zone-user mapping added for Resident services.
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/xlsx/registration_center.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/xlsx/registration_center.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="136">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -94,21 +94,60 @@
     <t xml:space="preserve">eng</t>
   </si>
   <si>
+    <t xml:space="preserve">10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual centre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual address 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual address 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MyCountry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23:59:59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(GTM+01:00) CENTRAL EUROPEAN TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fra</t>
+  </si>
+  <si>
     <t xml:space="preserve">Center A Ben Mansour</t>
   </si>
   <si>
-    <t xml:space="preserve">REG</t>
-  </si>
-  <si>
     <t xml:space="preserve">P4238</t>
   </si>
   <si>
     <t xml:space="preserve">Ben Mansour</t>
   </si>
   <si>
-    <t xml:space="preserve">MyCountry</t>
-  </si>
-  <si>
     <t xml:space="preserve">John Doe</t>
   </si>
   <si>
@@ -130,19 +169,7 @@
     <t xml:space="preserve">14:00:00</t>
   </si>
   <si>
-    <t xml:space="preserve">(GTM+01:00) CENTRAL EUROPEAN TIME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KTA</t>
-  </si>
-  <si>
     <t xml:space="preserve">RBT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fra</t>
   </si>
   <si>
     <t xml:space="preserve">Centre A Ben Mansour</t>
@@ -529,16 +556,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W33"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="R30" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W2" activeCellId="0" sqref="W2:W33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="8.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="16.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="40.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="9.02"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -616,41 +663,39 @@
       <c r="A2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>10001</v>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>34.52117</v>
+        <v>0</v>
       </c>
       <c r="I2" s="4" t="n">
-        <v>-6.453275</v>
+        <v>0</v>
       </c>
       <c r="J2" s="4" t="n">
-        <v>14022</v>
+        <v>0</v>
       </c>
       <c r="K2" s="4" t="n">
-        <v>779517433</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>29</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L2" s="4"/>
       <c r="M2" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>30</v>
@@ -665,63 +710,61 @@
         <v>33</v>
       </c>
       <c r="R2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="V2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="W2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>10001</v>
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>34.52117</v>
+        <v>0</v>
       </c>
       <c r="I3" s="4" t="n">
-        <v>-6.453275</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4" t="n">
-        <v>14022</v>
+        <v>0</v>
       </c>
       <c r="K3" s="4" t="n">
-        <v>993556086</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>29</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="L3" s="4"/>
       <c r="M3" s="4" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N3" s="4" t="s">
         <v>30</v>
@@ -736,22 +779,22 @@
         <v>33</v>
       </c>
       <c r="R3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T3" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U3" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V3" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,141 +802,141 @@
         <v>23</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>10002</v>
+        <v>10001</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>34.360207</v>
+        <v>34.52117</v>
       </c>
       <c r="I4" s="4" t="n">
-        <v>-6.550075</v>
+        <v>-6.453275</v>
       </c>
       <c r="J4" s="4" t="n">
-        <v>14053</v>
+        <v>14022</v>
       </c>
       <c r="K4" s="4" t="n">
-        <v>753476995</v>
+        <v>779517433</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M4" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V4" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>10001</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>10002</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="4" t="n">
+        <v>34.52117</v>
+      </c>
+      <c r="I5" s="4" t="n">
+        <v>-6.453275</v>
+      </c>
+      <c r="J5" s="4" t="n">
+        <v>14022</v>
+      </c>
+      <c r="K5" s="4" t="n">
+        <v>993556086</v>
+      </c>
+      <c r="L5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="4" t="n">
-        <v>34.360207</v>
-      </c>
-      <c r="I5" s="4" t="n">
-        <v>-6.550075</v>
-      </c>
-      <c r="J5" s="4" t="n">
-        <v>14053</v>
-      </c>
-      <c r="K5" s="4" t="n">
-        <v>984996886</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>47</v>
-      </c>
       <c r="M5" s="4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P5" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U5" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V5" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -901,141 +944,141 @@
         <v>23</v>
       </c>
       <c r="B6" s="1" t="n">
-        <v>10003</v>
+        <v>10002</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>34.405692</v>
+        <v>34.360207</v>
       </c>
       <c r="I6" s="4" t="n">
-        <v>-6.433368</v>
+        <v>-6.550075</v>
       </c>
       <c r="J6" s="4" t="n">
-        <v>14023</v>
+        <v>14053</v>
       </c>
       <c r="K6" s="4" t="n">
-        <v>734239083</v>
+        <v>753476995</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="M6" s="4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P6" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S6" s="4" t="s">
+      <c r="U6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U6" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V6" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="W6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>10003</v>
+        <v>10002</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>54</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="H7" s="4" t="n">
-        <v>34.405692</v>
+        <v>34.360207</v>
       </c>
       <c r="I7" s="4" t="n">
-        <v>-6.433368</v>
+        <v>-6.550075</v>
       </c>
       <c r="J7" s="4" t="n">
-        <v>14023</v>
+        <v>14053</v>
       </c>
       <c r="K7" s="4" t="n">
-        <v>675470523</v>
+        <v>984996886</v>
       </c>
       <c r="L7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="S7" s="4" t="s">
+      <c r="U7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U7" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V7" s="4" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="W7" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,141 +1086,141 @@
         <v>23</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>10004</v>
+        <v>10003</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>34.287879</v>
+        <v>34.405692</v>
       </c>
       <c r="I8" s="4" t="n">
-        <v>-6.516428</v>
+        <v>-6.433368</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>14000</v>
+        <v>14023</v>
       </c>
       <c r="K8" s="4" t="n">
-        <v>937997757</v>
+        <v>734239083</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="M8" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S8" s="4" t="s">
+      <c r="U8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U8" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V8" s="4" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>10004</v>
+        <v>10003</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>34.405692</v>
+      </c>
+      <c r="I9" s="4" t="n">
+        <v>-6.433368</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <v>14023</v>
+      </c>
+      <c r="K9" s="4" t="n">
+        <v>675470523</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>34.287879</v>
-      </c>
-      <c r="I9" s="4" t="n">
-        <v>-6.516428</v>
-      </c>
-      <c r="J9" s="4" t="n">
-        <v>14000</v>
-      </c>
-      <c r="K9" s="4" t="n">
-        <v>852492117</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="M9" s="4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P9" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q9" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U9" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V9" s="4" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1185,141 +1228,141 @@
         <v>23</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>10005</v>
+        <v>10004</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>34.256414</v>
+        <v>34.287879</v>
       </c>
       <c r="I10" s="4" t="n">
-        <v>-6.675499</v>
+        <v>-6.516428</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>14110</v>
+        <v>14000</v>
       </c>
       <c r="K10" s="4" t="n">
-        <v>887311749</v>
+        <v>937997757</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="M10" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q10" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S10" s="4" t="s">
+      <c r="U10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U10" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V10" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B11" s="1" t="n">
-        <v>10005</v>
+        <v>10004</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="4" t="n">
+        <v>34.287879</v>
+      </c>
+      <c r="I11" s="4" t="n">
+        <v>-6.516428</v>
+      </c>
+      <c r="J11" s="4" t="n">
+        <v>14000</v>
+      </c>
+      <c r="K11" s="4" t="n">
+        <v>852492117</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="4" t="n">
-        <v>34.256414</v>
-      </c>
-      <c r="I11" s="4" t="n">
-        <v>-6.675499</v>
-      </c>
-      <c r="J11" s="4" t="n">
-        <v>14110</v>
-      </c>
-      <c r="K11" s="4" t="n">
-        <v>658302699</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="M11" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P11" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q11" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V11" s="4" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1327,141 +1370,141 @@
         <v>23</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>10006</v>
+        <v>10005</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>34.262477</v>
+        <v>34.256414</v>
       </c>
       <c r="I12" s="4" t="n">
-        <v>-6.618605</v>
+        <v>-6.675499</v>
       </c>
       <c r="J12" s="4" t="n">
-        <v>14080</v>
+        <v>14110</v>
       </c>
       <c r="K12" s="4" t="n">
-        <v>915790305</v>
+        <v>887311749</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M12" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S12" s="4" t="s">
+      <c r="U12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T12" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V12" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>10006</v>
+        <v>10005</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H13" s="4" t="n">
-        <v>34.262477</v>
+        <v>34.256414</v>
       </c>
       <c r="I13" s="4" t="n">
-        <v>-6.618605</v>
+        <v>-6.675499</v>
       </c>
       <c r="J13" s="4" t="n">
-        <v>14080</v>
+        <v>14110</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>888439793</v>
+        <v>658302699</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="M13" s="4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P13" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q13" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U13" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V13" s="4" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,141 +1512,141 @@
         <v>23</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>10007</v>
+        <v>10006</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="H14" s="4" t="n">
-        <v>34.192861</v>
+        <v>34.262477</v>
       </c>
       <c r="I14" s="4" t="n">
-        <v>-6.683662</v>
+        <v>-6.618605</v>
       </c>
       <c r="J14" s="4" t="n">
-        <v>14025</v>
+        <v>14080</v>
       </c>
       <c r="K14" s="4" t="n">
-        <v>811552880</v>
+        <v>915790305</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M14" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P14" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q14" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R14" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S14" s="4" t="s">
+      <c r="U14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T14" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U14" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V14" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>10007</v>
+        <v>10006</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>34.262477</v>
+      </c>
+      <c r="I15" s="4" t="n">
+        <v>-6.618605</v>
+      </c>
+      <c r="J15" s="4" t="n">
+        <v>14080</v>
+      </c>
+      <c r="K15" s="4" t="n">
+        <v>888439793</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="4" t="n">
-        <v>34.192861</v>
-      </c>
-      <c r="I15" s="4" t="n">
-        <v>-6.683662</v>
-      </c>
-      <c r="J15" s="4" t="n">
-        <v>14025</v>
-      </c>
-      <c r="K15" s="4" t="n">
-        <v>753640112</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="M15" s="4" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O15" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P15" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T15" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V15" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1611,141 +1654,141 @@
         <v>23</v>
       </c>
       <c r="B16" s="1" t="n">
-        <v>10008</v>
+        <v>10007</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>34.522414</v>
+        <v>34.192861</v>
       </c>
       <c r="I16" s="4" t="n">
-        <v>-6.320471</v>
+        <v>-6.683662</v>
       </c>
       <c r="J16" s="4" t="n">
-        <v>14050</v>
+        <v>14025</v>
       </c>
       <c r="K16" s="4" t="n">
-        <v>695325692</v>
+        <v>811552880</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M16" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S16" s="4" t="s">
+      <c r="U16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U16" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V16" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1" t="n">
-        <v>10008</v>
+        <v>10007</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H17" s="4" t="n">
+        <v>34.192861</v>
+      </c>
+      <c r="I17" s="4" t="n">
+        <v>-6.683662</v>
+      </c>
+      <c r="J17" s="4" t="n">
+        <v>14025</v>
+      </c>
+      <c r="K17" s="4" t="n">
+        <v>753640112</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H17" s="4" t="n">
-        <v>34.522414</v>
-      </c>
-      <c r="I17" s="4" t="n">
-        <v>-6.320471</v>
-      </c>
-      <c r="J17" s="4" t="n">
-        <v>14050</v>
-      </c>
-      <c r="K17" s="4" t="n">
-        <v>862899075</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="M17" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N17" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P17" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U17" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="V17" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,141 +1796,141 @@
         <v>23</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>10009</v>
+        <v>10008</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>33.998232</v>
+        <v>34.522414</v>
       </c>
       <c r="I18" s="4" t="n">
-        <v>-6.845728</v>
+        <v>-6.320471</v>
       </c>
       <c r="J18" s="4" t="n">
-        <v>10106</v>
+        <v>14050</v>
       </c>
       <c r="K18" s="4" t="n">
-        <v>745360421</v>
+        <v>695325692</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="M18" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P18" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S18" s="4" t="s">
+      <c r="U18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T18" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="U18" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="V18" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="W18" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>10009</v>
+        <v>10008</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="4" t="n">
+        <v>34.522414</v>
+      </c>
+      <c r="I19" s="4" t="n">
+        <v>-6.320471</v>
+      </c>
+      <c r="J19" s="4" t="n">
+        <v>14050</v>
+      </c>
+      <c r="K19" s="4" t="n">
+        <v>862899075</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H19" s="4" t="n">
-        <v>33.998232</v>
-      </c>
-      <c r="I19" s="4" t="n">
-        <v>-6.845728</v>
-      </c>
-      <c r="J19" s="4" t="n">
-        <v>10106</v>
-      </c>
-      <c r="K19" s="4" t="n">
-        <v>676186831</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="M19" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P19" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q19" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="T19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U19" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="V19" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,141 +1938,141 @@
         <v>23</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>10010</v>
+        <v>10009</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>34.017502</v>
+        <v>33.998232</v>
       </c>
       <c r="I20" s="4" t="n">
-        <v>-6.834745</v>
+        <v>-6.845728</v>
       </c>
       <c r="J20" s="4" t="n">
-        <v>10000</v>
+        <v>10106</v>
       </c>
       <c r="K20" s="4" t="n">
-        <v>766074745</v>
+        <v>745360421</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M20" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N20" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O20" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P20" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R20" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S20" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T20" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U20" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V20" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W20" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>10010</v>
+        <v>10009</v>
       </c>
       <c r="C21" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="G21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="4" t="n">
+        <v>33.998232</v>
+      </c>
+      <c r="I21" s="4" t="n">
+        <v>-6.845728</v>
+      </c>
+      <c r="J21" s="4" t="n">
+        <v>10106</v>
+      </c>
+      <c r="K21" s="4" t="n">
+        <v>676186831</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="4" t="n">
-        <v>34.017502</v>
-      </c>
-      <c r="I21" s="4" t="n">
-        <v>-6.834745</v>
-      </c>
-      <c r="J21" s="4" t="n">
-        <v>10000</v>
-      </c>
-      <c r="K21" s="4" t="n">
-        <v>773606891</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>96</v>
       </c>
       <c r="M21" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P21" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V21" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W21" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2037,141 +2080,141 @@
         <v>23</v>
       </c>
       <c r="B22" s="1" t="n">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>33.986608</v>
+        <v>34.017502</v>
       </c>
       <c r="I22" s="4" t="n">
-        <v>-6.828873</v>
+        <v>-6.834745</v>
       </c>
       <c r="J22" s="4" t="n">
-        <v>10105</v>
+        <v>10000</v>
       </c>
       <c r="K22" s="4" t="n">
-        <v>787248921</v>
+        <v>766074745</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M22" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O22" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P22" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T22" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U22" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V22" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>10011</v>
+        <v>10010</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>34.017502</v>
+      </c>
+      <c r="I23" s="4" t="n">
+        <v>-6.834745</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>10000</v>
+      </c>
+      <c r="K23" s="4" t="n">
+        <v>773606891</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>105</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H23" s="4" t="n">
-        <v>33.986608</v>
-      </c>
-      <c r="I23" s="4" t="n">
-        <v>-6.828873</v>
-      </c>
-      <c r="J23" s="4" t="n">
-        <v>10105</v>
-      </c>
-      <c r="K23" s="4" t="n">
-        <v>878691008</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>102</v>
       </c>
       <c r="M23" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P23" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U23" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,141 +2222,141 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="n">
-        <v>10012</v>
+        <v>10011</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>33.978103</v>
+        <v>33.986608</v>
       </c>
       <c r="I24" s="4" t="n">
-        <v>-6.867849</v>
+        <v>-6.828873</v>
       </c>
       <c r="J24" s="4" t="n">
-        <v>10112</v>
+        <v>10105</v>
       </c>
       <c r="K24" s="4" t="n">
-        <v>838412388</v>
+        <v>787248921</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="M24" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P24" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T24" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T24" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U24" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="W24" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B25" s="1" t="n">
-        <v>10012</v>
+        <v>10011</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>33.978103</v>
+        <v>33.986608</v>
       </c>
       <c r="I25" s="4" t="n">
-        <v>-6.867849</v>
+        <v>-6.828873</v>
       </c>
       <c r="J25" s="4" t="n">
-        <v>10112</v>
+        <v>10105</v>
       </c>
       <c r="K25" s="4" t="n">
-        <v>719952201</v>
+        <v>878691008</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="M25" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P25" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q25" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R25" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="T25" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U25" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V25" s="4" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,141 +2364,141 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="n">
-        <v>10013</v>
+        <v>10012</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>33.953931</v>
+        <v>33.978103</v>
       </c>
       <c r="I26" s="4" t="n">
-        <v>-6.874735</v>
+        <v>-6.867849</v>
       </c>
       <c r="J26" s="4" t="n">
-        <v>10104</v>
+        <v>10112</v>
       </c>
       <c r="K26" s="4" t="n">
-        <v>751913644</v>
+        <v>838412388</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M26" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q26" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T26" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S26" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T26" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U26" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V26" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="n">
-        <v>10013</v>
+        <v>10012</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>33.953931</v>
+        <v>33.978103</v>
       </c>
       <c r="I27" s="4" t="n">
-        <v>-6.874735</v>
+        <v>-6.867849</v>
       </c>
       <c r="J27" s="4" t="n">
-        <v>10104</v>
+        <v>10112</v>
       </c>
       <c r="K27" s="4" t="n">
-        <v>956537434</v>
+        <v>719952201</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="M27" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q27" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U27" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V27" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,141 +2506,141 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="n">
-        <v>10014</v>
+        <v>10013</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H28" s="4" t="n">
-        <v>34.027757</v>
+        <v>33.953931</v>
       </c>
       <c r="I28" s="4" t="n">
-        <v>-6.834147</v>
+        <v>-6.874735</v>
       </c>
       <c r="J28" s="4" t="n">
-        <v>10036</v>
+        <v>10104</v>
       </c>
       <c r="K28" s="4" t="n">
-        <v>965639376</v>
+        <v>751913644</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M28" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O28" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q28" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R28" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T28" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S28" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T28" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U28" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V28" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1" t="n">
-        <v>10014</v>
+        <v>10013</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>34.027757</v>
+        <v>33.953931</v>
       </c>
       <c r="I29" s="4" t="n">
-        <v>-6.834147</v>
+        <v>-6.874735</v>
       </c>
       <c r="J29" s="4" t="n">
-        <v>10036</v>
+        <v>10104</v>
       </c>
       <c r="K29" s="4" t="n">
-        <v>781039430</v>
+        <v>956537434</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="M29" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q29" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2605,141 +2648,141 @@
         <v>23</v>
       </c>
       <c r="B30" s="1" t="n">
-        <v>10015</v>
+        <v>10014</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H30" s="4" t="n">
-        <v>33.995612</v>
+        <v>34.027757</v>
       </c>
       <c r="I30" s="4" t="n">
-        <v>-6.815281</v>
+        <v>-6.834147</v>
       </c>
       <c r="J30" s="4" t="n">
-        <v>10190</v>
+        <v>10036</v>
       </c>
       <c r="K30" s="4" t="n">
-        <v>803062069</v>
+        <v>965639376</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M30" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O30" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R30" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T30" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U30" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V30" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B31" s="1" t="n">
-        <v>10015</v>
+        <v>10014</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>33.995612</v>
+        <v>34.027757</v>
       </c>
       <c r="I31" s="4" t="n">
-        <v>-6.815281</v>
+        <v>-6.834147</v>
       </c>
       <c r="J31" s="4" t="n">
-        <v>10190</v>
+        <v>10036</v>
       </c>
       <c r="K31" s="4" t="n">
-        <v>731435978</v>
+        <v>781039430</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="M31" s="4" t="n">
         <v>2</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O31" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P31" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q31" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R31" s="4" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="S31" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="T31" s="4" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="U31" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V31" s="4" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2747,147 +2790,289 @@
         <v>23</v>
       </c>
       <c r="B32" s="1" t="n">
-        <v>33333</v>
+        <v>10015</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>33.52117</v>
+        <v>33.995612</v>
       </c>
       <c r="I32" s="4" t="n">
-        <v>-5.453275</v>
+        <v>-6.815281</v>
       </c>
       <c r="J32" s="4" t="n">
-        <v>14022</v>
+        <v>10190</v>
       </c>
       <c r="K32" s="4" t="n">
-        <v>779517433</v>
+        <v>803062069</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>29</v>
+        <v>132</v>
       </c>
       <c r="M32" s="4" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="O32" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="P32" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="R32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T32" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="S32" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T32" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="U32" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="V32" s="4" t="s">
-        <v>38</v>
+        <v>112</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>10015</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="4" t="n">
+        <v>33.995612</v>
+      </c>
+      <c r="I33" s="4" t="n">
+        <v>-6.815281</v>
+      </c>
+      <c r="J33" s="4" t="n">
+        <v>10190</v>
+      </c>
+      <c r="K33" s="4" t="n">
+        <v>731435978</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="M33" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q33" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T33" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V33" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>33333</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="1" t="n">
+      <c r="F34" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H34" s="4" t="n">
+        <v>33.52117</v>
+      </c>
+      <c r="I34" s="4" t="n">
+        <v>-5.453275</v>
+      </c>
+      <c r="J34" s="4" t="n">
+        <v>14022</v>
+      </c>
+      <c r="K34" s="4" t="n">
+        <v>779517433</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M34" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="N34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P34" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="1" t="n">
         <v>33333</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G33" s="4" t="s">
+      <c r="C35" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>33.52117</v>
+      </c>
+      <c r="I35" s="4" t="n">
+        <v>-5.453275</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>14022</v>
+      </c>
+      <c r="K35" s="4" t="n">
+        <v>993556086</v>
+      </c>
+      <c r="L35" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H33" s="4" t="n">
-        <v>33.52117</v>
-      </c>
-      <c r="I33" s="4" t="n">
-        <v>-5.453275</v>
-      </c>
-      <c r="J33" s="4" t="n">
-        <v>14022</v>
-      </c>
-      <c r="K33" s="4" t="n">
-        <v>993556086</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M33" s="4" t="n">
+      <c r="M35" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="N33" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O33" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q33" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="S33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="T33" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="U33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="V33" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="W33" s="1" t="s">
-        <v>39</v>
+      <c r="N35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="P35" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="R35" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="S35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="T35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="U35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="V35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="W35" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>